<commit_message>
commit full from server
</commit_message>
<xml_diff>
--- a/forms/shipping_plan/breakdown_container_print_xls.xlsx
+++ b/forms/shipping_plan/breakdown_container_print_xls.xlsx
@@ -23,16 +23,13 @@
     <t>ATTN :</t>
   </si>
   <si>
-    <t>PT. KLINE TOTAL LOGISTICS INDONESIA</t>
-  </si>
-  <si>
     <t>BOOKING NO. :</t>
   </si>
   <si>
     <t>FROM :</t>
   </si>
   <si>
-    <t xml:space="preserve"> - FDK INDONESIA</t>
+    <t>WISNU - FDK INDONESIA</t>
   </si>
   <si>
     <t>INVOICE NO. :</t>
@@ -47,7 +44,7 @@
     <t>PPBE NO. :</t>
   </si>
   <si>
-    <t>117/H/20</t>
+    <t>130/W/20</t>
   </si>
   <si>
     <t>VESSEL :</t>
@@ -101,20 +98,24 @@
     <t>VGM (KGS)</t>
   </si>
   <si>
-    <t>FI/20-153</t>
-  </si>
-  <si>
-    <t>AMAZON BASICS US LR6 (4SX2)</t>
-  </si>
-  <si>
-    <t>A
-(20 FEET)</t>
-  </si>
-  <si>
-    <t>AMAZON BASICS US LR6 (4SX5)</t>
+    <t>FIENR20-015</t>
+  </si>
+  <si>
+    <t>EVEREADY GOLD US LR6 BULK (E7075601)</t>
+  </si>
+  <si>
+    <t>E7075601</t>
+  </si>
+  <si>
+    <t>TGHU 5244 291 / ZZC-SB 109 121
+(40 FEET)</t>
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>TGHU 5245 488 / ZZC-SB 111 849
+(40 FEET)</t>
   </si>
   <si>
     <t>TOTAL ALL</t>
@@ -561,19 +562,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="43.560791" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13.85376" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="16.567383" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="11.425781" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="11.425781" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12.568359" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="12.568359" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="36.419678" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="21.137695" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="12.568359" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -600,14 +601,12 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
+      <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -616,16 +615,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -634,34 +633,34 @@
     </row>
     <row r="7" spans="1:13">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7"/>
       <c r="J7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:13">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -670,14 +669,14 @@
     </row>
     <row r="9" spans="1:13">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -686,189 +685,191 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12">
+        <v>52726</v>
+      </c>
+      <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="C12">
-        <v>88188</v>
-      </c>
-      <c r="D12"/>
       <c r="E12" s="3">
-        <v>25792</v>
+        <v>753920</v>
       </c>
       <c r="F12" s="3">
-        <v>124</v>
+        <v>1216</v>
       </c>
       <c r="G12" s="3">
-        <v>654.2</v>
+        <v>18452.8</v>
       </c>
       <c r="H12" s="3">
-        <v>669.6</v>
+        <v>17341.3</v>
       </c>
       <c r="I12" s="3">
-        <v>1.0752</v>
+        <v>14.1792</v>
       </c>
       <c r="J12" s="3">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="K12" t="s">
         <v>30</v>
       </c>
       <c r="L12" s="3">
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="M12" s="3">
-        <v>654.2</v>
+        <v>22152.8</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <v>88188</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13" s="3">
-        <v>50000</v>
-      </c>
-      <c r="F13" s="3">
-        <v>240.38461538</v>
-      </c>
-      <c r="G13" s="3">
-        <v>1308.4</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1301.4</v>
-      </c>
-      <c r="I13" s="3">
-        <v>1.9704</v>
-      </c>
-      <c r="J13" s="3">
-        <v>2</v>
-      </c>
-      <c r="K13"/>
-      <c r="L13" s="3">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
-        <v>1308.4</v>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5">
+        <v>753920</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1216</v>
+      </c>
+      <c r="G13" s="5">
+        <v>18452.8</v>
+      </c>
+      <c r="H13" s="5">
+        <v>17341.3</v>
+      </c>
+      <c r="I13" s="5">
+        <v>14.179</v>
+      </c>
+      <c r="J13" s="5">
+        <v>19</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="5">
+        <v>3700</v>
+      </c>
+      <c r="M13" s="5">
+        <v>22152.8</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
       <c r="C14">
-        <v>88918</v>
-      </c>
-      <c r="D14"/>
+        <v>52726</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
       <c r="E14" s="3">
-        <v>221000</v>
+        <v>753920</v>
       </c>
       <c r="F14" s="3">
-        <v>425</v>
+        <v>1216</v>
       </c>
       <c r="G14" s="3">
-        <v>6188.6</v>
+        <v>18452.8</v>
       </c>
       <c r="H14" s="3">
-        <v>5610</v>
+        <v>17341.3</v>
       </c>
       <c r="I14" s="3">
-        <v>8.683199999999999</v>
+        <v>14.1792</v>
       </c>
       <c r="J14" s="3">
-        <v>12</v>
-      </c>
-      <c r="K14"/>
+        <v>19</v>
+      </c>
+      <c r="K14" t="s">
+        <v>32</v>
+      </c>
       <c r="L14" s="3">
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="M14" s="3">
-        <v>6188.6</v>
+        <v>22152.8</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5">
-        <v>296792</v>
+        <v>753920</v>
       </c>
       <c r="F15" s="5">
-        <v>789.38461538</v>
+        <v>1216</v>
       </c>
       <c r="G15" s="5">
-        <v>8151.200000000001</v>
+        <v>18452.8</v>
       </c>
       <c r="H15" s="5">
-        <v>7581</v>
+        <v>17341.3</v>
       </c>
       <c r="I15" s="5">
-        <v>11.728</v>
+        <v>14.179</v>
       </c>
       <c r="J15" s="5">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="5">
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="M15" s="5">
-        <v>8151.200000000001</v>
+        <v>22152.8</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -879,29 +880,29 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7">
-        <v>296792</v>
+        <v>1507840</v>
       </c>
       <c r="F17" s="7">
-        <v>789.38461538</v>
+        <v>2432</v>
       </c>
       <c r="G17" s="7">
-        <v>8151.200000000001</v>
+        <v>36905.6</v>
       </c>
       <c r="H17" s="7">
-        <v>7581</v>
+        <v>34682.6</v>
       </c>
       <c r="I17" s="7">
-        <v>11.728</v>
+        <v>28.358</v>
       </c>
       <c r="J17" s="7">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="7">
-        <v>0</v>
+        <v>7400</v>
       </c>
       <c r="M17" s="7">
-        <v>8151.200000000001</v>
+        <v>44305.6</v>
       </c>
     </row>
   </sheetData>
@@ -923,6 +924,8 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:L9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="A17:B17"/>

</xml_diff>